<commit_message>
Atualizada documentação de projeto, validadores
</commit_message>
<xml_diff>
--- a/Projeto/2 - Levantamento de requisitos/3 - Matriz de rastreabilidade/Matriz de rastreabilidade de requisitos.xlsx
+++ b/Projeto/2 - Levantamento de requisitos/3 - Matriz de rastreabilidade/Matriz de rastreabilidade de requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\NetBeansProjects\genesys-petshop\Projeto\2 - Levantamento de requisitos\3 - Matriz de rastreabilidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B80D162-F747-4820-B2A9-9C3EC3BD7344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37C693E-3BC2-4DEC-9924-EE77122DF505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t>Matriz de rastreabilidade de requisitos</t>
   </si>
@@ -125,13 +125,16 @@
   </si>
   <si>
     <t>UC-022 Configurar conexão remota</t>
+  </si>
+  <si>
+    <t>Revisado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -240,7 +243,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +298,12 @@
         <bgColor rgb="FF77BC65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -341,7 +350,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -360,6 +369,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -396,9 +408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -436,7 +448,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -542,7 +554,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -684,7 +696,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,23 +706,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="1023" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="1023" width="12.140625" style="1" customWidth="1"/>
     <col min="1024" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -719,16 +731,18 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -736,7 +750,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -755,8 +769,11 @@
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -764,7 +781,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -783,8 +800,11 @@
       <c r="F6" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -803,8 +823,11 @@
       <c r="F7" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -823,8 +846,9 @@
       <c r="F8" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -843,8 +867,11 @@
       <c r="F9" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -863,8 +890,9 @@
       <c r="F10" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -883,8 +911,11 @@
       <c r="F11" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -903,8 +934,11 @@
       <c r="F12" s="3">
         <v>44833</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -923,8 +957,11 @@
       <c r="F13" s="3">
         <v>44811</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -943,8 +980,11 @@
       <c r="F14" s="3">
         <v>44834</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -963,8 +1003,11 @@
       <c r="F15" s="3">
         <v>44804</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -983,8 +1026,9 @@
       <c r="F16" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1003,8 +1047,9 @@
       <c r="F17" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1023,8 +1068,11 @@
       <c r="F18" s="3">
         <v>44788</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1043,8 +1091,11 @@
       <c r="F19" s="3">
         <v>44805</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="3">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1063,8 +1114,9 @@
       <c r="F20" s="3">
         <v>44789</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1083,8 +1135,11 @@
       <c r="F21" s="3">
         <v>44789</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1103,8 +1158,9 @@
       <c r="F22" s="3">
         <v>44811</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1123,8 +1179,9 @@
       <c r="F23" s="3">
         <v>44811</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1143,8 +1200,9 @@
       <c r="F24" s="3">
         <v>44835</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1163,8 +1221,9 @@
       <c r="F25" s="3">
         <v>44848</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1183,8 +1242,11 @@
       <c r="F26" s="3">
         <v>44847</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="1" customFormat="1">
+      <c r="G26" s="3">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1203,14 +1265,18 @@
       <c r="F27" s="3">
         <v>45142</v>
       </c>
+      <c r="G27" s="3">
+        <v>45759</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A1:G2"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>

</xml_diff>